<commit_message>
organized excel and added extend properties
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/BookStoreApi.xlsx
+++ b/src/test/resources/testData/BookStoreApi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudha\Documents\Sudha\Sudha_Studies\NumpyNinja_QA_Automation\Api_Testing\ApiPractice_Myself\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2A45E8-B606-4832-8072-9A10EB5D141C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E43EE60-49B9-40E2-B9AD-C475884E1CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{2672C68F-A1B1-4BAD-8A98-150D8F1636BA}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>TestScenario</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>bookTest272</t>
+  </si>
+  <si>
+    <t>TestCases</t>
   </si>
 </sst>
 </file>
@@ -910,62 +910,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EEE263-F3D0-407C-BB1F-81A0D9ED0184}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
       <c r="G2">
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>